<commit_message>
Added References/Covariance and State Estimation.pdf
</commit_message>
<xml_diff>
--- a/References/Literature Review.xlsx
+++ b/References/Literature Review.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_Main\trunk\References\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1320" windowWidth="25060" windowHeight="17040" tabRatio="649"/>
+    <workbookView xWindow="1740" yWindow="1320" windowWidth="25065" windowHeight="17040" tabRatio="649"/>
   </bookViews>
   <sheets>
     <sheet name="Complete List" sheetId="10" r:id="rId1"/>
@@ -480,7 +485,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -549,7 +554,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -595,6 +600,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -604,7 +615,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -617,6 +630,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -945,54 +966,57 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="16"/>
+    <col min="4" max="4" width="5.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="83.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="109.25" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="11" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="C2" t="s">
+    <row r="2" spans="1:6" ht="31.5">
+      <c r="C2" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="16">
         <v>2006</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="15" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1007,7 +1031,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1026,11 +1050,11 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="102.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="102.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1048,7 +1072,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1062,7 +1086,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="15"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1074,23 +1098,23 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="15"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="15"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:5" s="15" customFormat="1"/>
+    <row r="8" spans="1:5" s="17" customFormat="1"/>
     <row r="9" spans="1:5">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1104,7 +1128,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="15"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
@@ -1113,7 +1137,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="15"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1121,9 +1145,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="15" customFormat="1"/>
+    <row r="12" spans="1:5" s="17" customFormat="1"/>
     <row r="13" spans="1:5">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1137,7 +1161,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="15"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1149,23 +1173,23 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1">
-      <c r="A15" s="15"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="19">
-      <c r="A16" s="15"/>
+    <row r="16" spans="1:5" ht="20.25">
+      <c r="A16" s="17"/>
       <c r="B16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="15"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="5"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:5" s="15" customFormat="1"/>
+    <row r="18" spans="1:5" s="17" customFormat="1"/>
     <row r="19" spans="1:5">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1182,24 +1206,24 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="15"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="15"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="15"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="15"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:5" s="15" customFormat="1"/>
+    <row r="24" spans="1:5" s="17" customFormat="1"/>
     <row r="25" spans="1:5">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="17" t="s">
         <v>50</v>
       </c>
       <c r="D25" t="s">
@@ -1207,62 +1231,62 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="15"/>
+      <c r="A26" s="17"/>
       <c r="D26" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="15"/>
+      <c r="A27" s="17"/>
       <c r="D27" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="15"/>
+      <c r="A28" s="17"/>
       <c r="D28" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="15"/>
+      <c r="A29" s="17"/>
       <c r="D29" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="15"/>
+      <c r="A30" s="17"/>
       <c r="D30" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="15"/>
+      <c r="A31" s="17"/>
       <c r="D31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="15"/>
+      <c r="A32" s="17"/>
       <c r="D32" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="15"/>
+      <c r="A33" s="17"/>
       <c r="D33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="15"/>
+      <c r="A34" s="17"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="15"/>
-    </row>
-    <row r="36" spans="1:4" s="15" customFormat="1"/>
+      <c r="A35" s="17"/>
+    </row>
+    <row r="36" spans="1:4" s="17" customFormat="1"/>
     <row r="37" spans="1:4">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="17" t="s">
         <v>51</v>
       </c>
       <c r="B37" s="7" t="s">
@@ -1273,36 +1297,36 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="15"/>
+      <c r="A38" s="17"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="15"/>
+      <c r="A39" s="17"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="15"/>
+      <c r="A40" s="17"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="15"/>
+      <c r="A41" s="17"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="15"/>
+      <c r="A42" s="17"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="15"/>
+      <c r="A43" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A25:A35"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A24:XFD24"/>
     <mergeCell ref="A36:XFD36"/>
     <mergeCell ref="A8:XFD8"/>
     <mergeCell ref="A12:XFD12"/>
     <mergeCell ref="A18:XFD18"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A25:A35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1322,7 +1346,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
   </cols>
@@ -1333,7 +1357,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1341,28 +1365,28 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
       <c r="B3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="16"/>
+      <c r="A5" s="18"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -1370,31 +1394,31 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="16"/>
+      <c r="A9" s="18"/>
       <c r="B9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="18"/>
       <c r="B10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="16"/>
+      <c r="A11" s="18"/>
       <c r="B11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="16"/>
+      <c r="A12" s="18"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B14" t="s">
@@ -1402,31 +1426,31 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="16"/>
+      <c r="A15" s="18"/>
       <c r="B15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="16"/>
+      <c r="A16" s="18"/>
       <c r="B16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="16"/>
+      <c r="A17" s="18"/>
       <c r="B17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="16"/>
+      <c r="A18" s="18"/>
       <c r="B18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="16"/>
+      <c r="A19" s="18"/>
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -1435,7 +1459,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
@@ -1443,31 +1467,31 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="16"/>
+      <c r="A22" s="18"/>
       <c r="B22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="16"/>
+      <c r="A23" s="18"/>
       <c r="B23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="16"/>
+      <c r="A24" s="18"/>
       <c r="B24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="16"/>
+      <c r="A25" s="18"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B27" t="s">
@@ -1475,25 +1499,25 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="16"/>
+      <c r="A28" s="18"/>
       <c r="B28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="16"/>
+      <c r="A29" s="18"/>
       <c r="B29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="16"/>
+      <c r="A30" s="18"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="16"/>
+      <c r="A31" s="18"/>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="16"/>
+      <c r="A32" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1520,61 +1544,61 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="16"/>
+      <c r="A2" s="18"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="16"/>
+      <c r="A5" s="18"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="16"/>
+      <c r="A7" s="18"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="16"/>
+      <c r="A8" s="18"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="16"/>
+      <c r="A9" s="18"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="16"/>
+      <c r="A10" s="18"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="17" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="15"/>
+      <c r="A12" s="17"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="15"/>
+      <c r="A13" s="17"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="15"/>
+      <c r="A14" s="17"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="15"/>
+      <c r="A15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1597,7 +1621,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1616,9 +1640,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="95.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="95.875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="96" customHeight="1">
@@ -1626,7 +1650,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="94" customHeight="1">
+    <row r="2" spans="1:1" ht="93.95" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>54</v>
       </c>
@@ -1655,12 +1679,12 @@
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="7"/>
+    <col min="2" max="2" width="46.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="7"/>
     <col min="5" max="5" width="13" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1679,7 +1703,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B2" t="s">
@@ -1696,7 +1720,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="18"/>
+      <c r="A3" s="20"/>
       <c r="B3" t="s">
         <v>72</v>
       </c>
@@ -1711,7 +1735,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="18"/>
+      <c r="A4" s="20"/>
       <c r="B4" t="s">
         <v>74</v>
       </c>
@@ -1726,7 +1750,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18"/>
+      <c r="A5" s="20"/>
       <c r="B5" t="s">
         <v>75</v>
       </c>
@@ -1741,7 +1765,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="18"/>
+      <c r="A6" s="20"/>
       <c r="B6" t="s">
         <v>76</v>
       </c>
@@ -1756,7 +1780,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="18"/>
+      <c r="A7" s="20"/>
       <c r="B7" t="s">
         <v>77</v>
       </c>
@@ -1770,9 +1794,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="18" customFormat="1"/>
+    <row r="8" spans="1:5" s="20" customFormat="1"/>
     <row r="9" spans="1:5">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="20" t="s">
         <v>84</v>
       </c>
       <c r="B9" t="s">
@@ -1783,7 +1807,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="18"/>
+      <c r="A10" s="20"/>
       <c r="B10" t="s">
         <v>80</v>
       </c>
@@ -1792,7 +1816,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="18"/>
+      <c r="A11" s="20"/>
       <c r="B11" t="s">
         <v>81</v>
       </c>
@@ -1801,7 +1825,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="18"/>
+      <c r="A12" s="20"/>
       <c r="B12" t="s">
         <v>82</v>
       </c>
@@ -1816,7 +1840,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="18"/>
+      <c r="A13" s="20"/>
       <c r="B13" t="s">
         <v>83</v>
       </c>
@@ -1831,7 +1855,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="18"/>
+      <c r="A14" s="20"/>
       <c r="B14" t="s">
         <v>77</v>
       </c>
@@ -1845,9 +1869,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="19" customFormat="1"/>
+    <row r="15" spans="1:5" s="21" customFormat="1"/>
     <row r="16" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="20" t="s">
         <v>94</v>
       </c>
       <c r="B16" t="s">
@@ -1864,7 +1888,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="18"/>
+      <c r="A17" s="20"/>
       <c r="B17" t="s">
         <v>86</v>
       </c>
@@ -1879,7 +1903,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="18"/>
+      <c r="A18" s="20"/>
       <c r="B18" t="s">
         <v>87</v>
       </c>
@@ -1894,7 +1918,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="18"/>
+      <c r="A19" s="20"/>
       <c r="B19" t="s">
         <v>89</v>
       </c>
@@ -1909,7 +1933,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="18"/>
+      <c r="A20" s="20"/>
       <c r="B20" t="s">
         <v>91</v>
       </c>
@@ -1924,7 +1948,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="18"/>
+      <c r="A21" s="20"/>
       <c r="B21" t="s">
         <v>93</v>
       </c>
@@ -1938,9 +1962,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="19" customFormat="1"/>
+    <row r="22" spans="1:5" s="21" customFormat="1"/>
     <row r="23" spans="1:5" s="7" customFormat="1">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="20" t="s">
         <v>117</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -1957,7 +1981,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A24" s="18"/>
+      <c r="A24" s="20"/>
       <c r="B24" t="s">
         <v>95</v>
       </c>
@@ -1972,7 +1996,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="18"/>
+      <c r="A25" s="20"/>
       <c r="B25" t="s">
         <v>115</v>
       </c>
@@ -1987,7 +2011,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="18"/>
+      <c r="A26" s="20"/>
       <c r="B26" t="s">
         <v>77</v>
       </c>
@@ -2002,7 +2026,7 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="18"/>
+      <c r="A27" s="20"/>
       <c r="B27" t="s">
         <v>97</v>
       </c>
@@ -2017,11 +2041,11 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="18"/>
-    </row>
-    <row r="29" spans="1:5" s="19" customFormat="1"/>
+      <c r="A28" s="20"/>
+    </row>
+    <row r="29" spans="1:5" s="21" customFormat="1"/>
     <row r="30" spans="1:5" s="7" customFormat="1">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="20" t="s">
         <v>104</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -2038,7 +2062,7 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="18"/>
+      <c r="A31" s="20"/>
       <c r="B31" t="s">
         <v>101</v>
       </c>
@@ -2053,7 +2077,7 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="18"/>
+      <c r="A32" s="20"/>
       <c r="B32" t="s">
         <v>118</v>
       </c>
@@ -2068,7 +2092,7 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="18"/>
+      <c r="A33" s="20"/>
       <c r="B33" t="s">
         <v>103</v>
       </c>
@@ -2082,9 +2106,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="19" customFormat="1"/>
+    <row r="34" spans="1:5" s="21" customFormat="1"/>
     <row r="35" spans="1:5" s="7" customFormat="1">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="20" t="s">
         <v>106</v>
       </c>
       <c r="B35" t="s">
@@ -2101,7 +2125,7 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="18"/>
+      <c r="A36" s="20"/>
       <c r="B36" t="s">
         <v>105</v>
       </c>
@@ -2116,7 +2140,7 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="18"/>
+      <c r="A37" s="20"/>
       <c r="B37" t="s">
         <v>122</v>
       </c>
@@ -2130,7 +2154,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="19" customFormat="1"/>
+    <row r="38" spans="1:5" s="21" customFormat="1"/>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>109</v>
@@ -2148,9 +2172,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="19" customFormat="1"/>
+    <row r="40" spans="1:5" s="21" customFormat="1"/>
     <row r="41" spans="1:5">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="19" t="s">
         <v>123</v>
       </c>
       <c r="B41" t="s">
@@ -2167,7 +2191,7 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="17"/>
+      <c r="A42" s="19"/>
       <c r="B42" t="s">
         <v>111</v>
       </c>
@@ -2182,7 +2206,7 @@
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="17"/>
+      <c r="A43" s="19"/>
       <c r="B43" t="s">
         <v>112</v>
       </c>
@@ -2308,11 +2332,11 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.875" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2349,47 +2373,47 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="80.5" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>138</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45">
-      <c r="A2" s="18"/>
+    <row r="2" spans="1:2" ht="47.25">
+      <c r="A2" s="20"/>
       <c r="B2" s="14" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="18"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="12"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="18"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="13"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="18"/>
+      <c r="A5" s="20"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="20"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="18"/>
+      <c r="A7" s="20"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="18"/>
+      <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="18"/>
+      <c r="A9" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>